<commit_message>
Updated requirements and value maps
</commit_message>
<xml_diff>
--- a/valid_values_map.xlsx
+++ b/valid_values_map.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="131">
   <si>
     <t>Code</t>
   </si>
@@ -764,7 +764,7 @@
   <dimension ref="A1:J64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,12 +896,7 @@
       <c r="C5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>98</v>
-      </c>
+      <c r="D5" s="5"/>
       <c r="F5" s="3" t="s">
         <v>98</v>
       </c>
@@ -964,12 +959,7 @@
       <c r="C8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>98</v>
-      </c>
+      <c r="D8" s="5"/>
       <c r="F8" s="3" t="s">
         <v>98</v>
       </c>

</xml_diff>

<commit_message>
3 year IBC/SRS approvals. Support for Scientific Review
</commit_message>
<xml_diff>
--- a/valid_values_map.xlsx
+++ b/valid_values_map.xlsx
@@ -15,7 +15,7 @@
     <sheet name="values" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">values!$A$1:$J$64</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">values!$A$1:$J$65</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="133">
   <si>
     <t>Code</t>
   </si>
@@ -420,6 +420,12 @@
   </si>
   <si>
     <t>MMR</t>
+  </si>
+  <si>
+    <t>Scientific Review</t>
+  </si>
+  <si>
+    <t>Research - Not Engaged</t>
   </si>
 </sst>
 </file>
@@ -761,10 +767,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J64"/>
+  <dimension ref="A1:K65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,7 +782,7 @@
     <col min="6" max="10" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>93</v>
       </c>
@@ -807,8 +813,11 @@
       <c r="J1" s="4" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>70</v>
       </c>
@@ -839,8 +848,11 @@
       <c r="J2" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>70</v>
       </c>
@@ -860,7 +872,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>70</v>
       </c>
@@ -886,7 +898,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>70</v>
       </c>
@@ -907,7 +919,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>70</v>
       </c>
@@ -922,7 +934,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>70</v>
       </c>
@@ -948,8 +960,11 @@
       <c r="J7" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>70</v>
       </c>
@@ -964,7 +979,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>70</v>
       </c>
@@ -988,7 +1003,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>100</v>
       </c>
@@ -1019,8 +1034,11 @@
       <c r="J10" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>100</v>
       </c>
@@ -1039,8 +1057,11 @@
       <c r="F11" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>100</v>
       </c>
@@ -1071,8 +1092,11 @@
       <c r="J12" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>100</v>
       </c>
@@ -1103,8 +1127,11 @@
       <c r="J13" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>100</v>
       </c>
@@ -1127,8 +1154,11 @@
       <c r="J14" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>100</v>
       </c>
@@ -1153,8 +1183,11 @@
       <c r="I15" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>100</v>
       </c>
@@ -1185,8 +1218,11 @@
       <c r="J16" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>100</v>
       </c>
@@ -1217,8 +1253,11 @@
       <c r="J17" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>100</v>
       </c>
@@ -1249,8 +1288,11 @@
       <c r="J18" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>100</v>
       </c>
@@ -1272,8 +1314,11 @@
       <c r="G19" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>100</v>
       </c>
@@ -1287,8 +1332,11 @@
       <c r="F20" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>100</v>
       </c>
@@ -1314,8 +1362,11 @@
       <c r="J21" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>100</v>
       </c>
@@ -1346,8 +1397,11 @@
       <c r="J22" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>100</v>
       </c>
@@ -1378,8 +1432,11 @@
       <c r="J23" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>100</v>
       </c>
@@ -1405,8 +1462,11 @@
       <c r="J24" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>100</v>
       </c>
@@ -1437,8 +1497,11 @@
       <c r="J25" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>100</v>
       </c>
@@ -1469,54 +1532,57 @@
       <c r="J26" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>100</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D27" s="5"/>
-      <c r="J27" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>98</v>
-      </c>
+      <c r="D28" s="5"/>
       <c r="J28" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>98</v>
@@ -1530,16 +1596,19 @@
       <c r="J29" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K29" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>20</v>
+        <v>122</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>98</v>
@@ -1553,16 +1622,19 @@
       <c r="J30" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K30" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>123</v>
+        <v>20</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>98</v>
@@ -1576,16 +1648,19 @@
       <c r="J31" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K31" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>98</v>
@@ -1599,16 +1674,19 @@
       <c r="J32" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K32" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>98</v>
@@ -1619,28 +1697,22 @@
       <c r="F33" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="G33" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="J33" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K33" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>98</v>
@@ -1663,16 +1735,19 @@
       <c r="J34" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K34" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>98</v>
@@ -1695,16 +1770,19 @@
       <c r="J35" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K35" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>98</v>
@@ -1727,16 +1805,19 @@
       <c r="J36" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K36" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>125</v>
+        <v>22</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>98</v>
@@ -1759,16 +1840,19 @@
       <c r="J37" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K37" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>98</v>
@@ -1791,16 +1875,19 @@
       <c r="J38" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K38" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>98</v>
@@ -1823,16 +1910,19 @@
       <c r="J39" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K39" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>98</v>
@@ -1843,16 +1933,31 @@
       <c r="F40" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G40" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>98</v>
@@ -1863,22 +1968,19 @@
       <c r="F41" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="H41" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="I41" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K41" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>98</v>
@@ -1889,21 +1991,27 @@
       <c r="F42" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="G42" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H42" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C43" t="s">
-        <v>81</v>
-      </c>
-      <c r="D43" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D43" s="5" t="s">
         <v>98</v>
       </c>
       <c r="E43" s="3" t="s">
@@ -1912,18 +2020,24 @@
       <c r="F43" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G43" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="K43" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D44" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" t="s">
+        <v>81</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>98</v>
       </c>
       <c r="E44" s="3" t="s">
@@ -1932,16 +2046,19 @@
       <c r="F44" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K44" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>117</v>
+        <v>63</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>98</v>
@@ -1952,28 +2069,19 @@
       <c r="F45" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="G45" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="I45" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="J45" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K45" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>98</v>
@@ -1996,49 +2104,55 @@
       <c r="J46" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K46" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="K47" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D47" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="I47" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="J47" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="D48" s="5" t="s">
         <v>98</v>
       </c>
@@ -2048,38 +2162,53 @@
       <c r="F48" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G48" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>102</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D49" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B50" t="s">
-        <v>6</v>
-      </c>
-      <c r="C50" t="s">
-        <v>7</v>
-      </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" s="5" t="s">
         <v>98</v>
       </c>
       <c r="E50" s="3" t="s">
@@ -2088,19 +2217,19 @@
       <c r="F50" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="J50" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K50" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>103</v>
       </c>
       <c r="B51" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C51" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>98</v>
@@ -2111,28 +2240,22 @@
       <c r="F51" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="G51" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="H51" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="I51" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="J51" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K51" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>103</v>
       </c>
       <c r="B52" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C52" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>98</v>
@@ -2155,16 +2278,19 @@
       <c r="J52" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K52" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>103</v>
       </c>
       <c r="B53" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C53" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>98</v>
@@ -2187,16 +2313,19 @@
       <c r="J53" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K53" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>103</v>
       </c>
       <c r="B54" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C54" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>98</v>
@@ -2219,16 +2348,19 @@
       <c r="J54" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K54" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>103</v>
       </c>
       <c r="B55" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C55" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>98</v>
@@ -2251,16 +2383,19 @@
       <c r="J55" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K55" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>103</v>
       </c>
       <c r="B56" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C56" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>98</v>
@@ -2283,16 +2418,19 @@
       <c r="J56" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K56" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>103</v>
       </c>
       <c r="B57" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C57" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>98</v>
@@ -2303,6 +2441,9 @@
       <c r="F57" s="3" t="s">
         <v>98</v>
       </c>
+      <c r="G57" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="H57" s="3" t="s">
         <v>98</v>
       </c>
@@ -2312,16 +2453,19 @@
       <c r="J57" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K57" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>103</v>
       </c>
       <c r="B58" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C58" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>98</v>
@@ -2341,16 +2485,19 @@
       <c r="J58" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K58" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>103</v>
       </c>
       <c r="B59" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C59" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>98</v>
@@ -2361,22 +2508,28 @@
       <c r="F59" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="G59" s="3" t="s">
+      <c r="H59" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I59" s="3" t="s">
         <v>98</v>
       </c>
       <c r="J59" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K59" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>103</v>
       </c>
       <c r="B60" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C60" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>98</v>
@@ -2390,25 +2543,22 @@
       <c r="G60" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="H60" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="I60" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="J60" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K60" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>103</v>
       </c>
       <c r="B61" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C61" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>98</v>
@@ -2431,16 +2581,19 @@
       <c r="J61" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K61" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>103</v>
       </c>
       <c r="B62" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C62" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>98</v>
@@ -2451,42 +2604,80 @@
       <c r="F62" s="3" t="s">
         <v>98</v>
       </c>
+      <c r="G62" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I62" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="J62" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K62" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>103</v>
       </c>
       <c r="B63" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="C63" t="s">
-        <v>86</v>
-      </c>
-      <c r="D63" s="3"/>
-      <c r="G63" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="J63" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="K63" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>103</v>
       </c>
       <c r="B64" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C64" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D64" s="3"/>
       <c r="G64" s="3" t="s">
         <v>98</v>
       </c>
     </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B65" t="s">
+        <v>90</v>
+      </c>
+      <c r="C65" t="s">
+        <v>91</v>
+      </c>
+      <c r="D65" s="3"/>
+      <c r="G65" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J64"/>
+  <autoFilter ref="A1:J65"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New sub type TRI and action RNE
</commit_message>
<xml_diff>
--- a/valid_values_map.xlsx
+++ b/valid_values_map.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="135">
   <si>
     <t>Code</t>
   </si>
@@ -426,6 +426,12 @@
   </si>
   <si>
     <t>Research - Not Engaged</t>
+  </si>
+  <si>
+    <t>TRI</t>
+  </si>
+  <si>
+    <t>Triennial Review</t>
   </si>
 </sst>
 </file>
@@ -767,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K65"/>
+  <dimension ref="A1:K66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2676,8 +2682,23 @@
         <v>98</v>
       </c>
     </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B66" t="s">
+        <v>134</v>
+      </c>
+      <c r="C66" t="s">
+        <v>133</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:J65"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>